<commit_message>
scale data to match units
</commit_message>
<xml_diff>
--- a/spreadsheet_conversion/blood/blood_example.xlsx
+++ b/spreadsheet_conversion/blood/blood_example.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25601"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25629"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cpernet\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\BIDS\ONP\BIDS-converter\spreadsheet_conversion\blood\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05BD7794-070C-4DC3-99A4-001F7CEBBFF3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E15331A8-5862-47A9-8BC0-5EB783ED4BCE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10560" xr2:uid="{B09AB50C-E81C-BF4B-AB80-4C0F8EC55ACD}"/>
   </bookViews>
@@ -533,7 +533,7 @@
   <dimension ref="A1:AD26"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="X1" workbookViewId="0">
-      <selection activeCell="AC26" sqref="AC26"/>
+      <selection activeCell="Y30" sqref="Y30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
@@ -843,6 +843,7 @@
       <c r="AB10">
         <v>19.430288690813679</v>
       </c>
+      <c r="AD10" s="3"/>
     </row>
     <row r="11" spans="1:30" x14ac:dyDescent="0.35">
       <c r="X11">
@@ -857,13 +858,13 @@
         <v>5</v>
       </c>
       <c r="Y12">
-        <v>0.94240185871412085</v>
+        <v>2.6038257396855347</v>
       </c>
       <c r="Z12">
-        <v>0.94240185871412085</v>
+        <v>2.6038257396855347</v>
       </c>
       <c r="AA12">
-        <v>0.87597377200000004</v>
+        <v>2.4202870927432429</v>
       </c>
       <c r="AB12">
         <v>2.6038257396855387</v>
@@ -957,13 +958,10 @@
         <v>1510878819</v>
       </c>
       <c r="Z23">
-        <v>0.88717388582392775</v>
+        <v>2.4512326436167768</v>
       </c>
       <c r="AA23">
-        <v>0.73078032900000001</v>
-      </c>
-      <c r="AB23">
-        <v>1.5108788193035168</v>
+        <v>2.0191223235726747</v>
       </c>
     </row>
     <row r="24" spans="24:28" x14ac:dyDescent="0.35">
@@ -974,13 +972,10 @@
         <v>1250953944</v>
       </c>
       <c r="Z24">
-        <v>0.9876970497706401</v>
+        <v>2.7289748820247333</v>
       </c>
       <c r="AA24">
-        <v>0.48267500400000002</v>
-      </c>
-      <c r="AB24">
-        <v>1.2509539442295483</v>
+        <v>1.3336153655648415</v>
       </c>
     </row>
     <row r="25" spans="24:28" x14ac:dyDescent="0.35">
@@ -991,13 +986,10 @@
         <v>1302358278</v>
       </c>
       <c r="Z25">
-        <v>1.0607712243826037</v>
+        <v>2.9308764540574193</v>
       </c>
       <c r="AA25">
-        <v>0.25832960100000002</v>
-      </c>
-      <c r="AB25">
-        <v>1.3023582780919436</v>
+        <v>0.71375630065532591</v>
       </c>
     </row>
     <row r="26" spans="24:28" x14ac:dyDescent="0.35">
@@ -1008,13 +1000,10 @@
         <v>1363570232</v>
       </c>
       <c r="Z26">
-        <v>1.1914855637010808</v>
+        <v>3.2920359298333337</v>
       </c>
       <c r="AA26">
-        <v>0.14819046799999999</v>
-      </c>
-      <c r="AB26">
-        <v>1.3635702323215919</v>
+        <v>0.40944545194439969</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add a metadata column
</commit_message>
<xml_diff>
--- a/spreadsheet_conversion/blood/blood_example.xlsx
+++ b/spreadsheet_conversion/blood/blood_example.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\BIDS\ONP\BIDS-converter\spreadsheet_conversion\blood\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B719E53-6A28-4349-8EB9-E975DCB41218}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E88A1DCB-DBD0-43FA-9921-F3597D3BE255}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10560" xr2:uid="{B09AB50C-E81C-BF4B-AB80-4C0F8EC55ACD}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="49">
   <si>
     <t>Manufacturer</t>
   </si>
@@ -167,6 +167,21 @@
   </si>
   <si>
     <t>time_manual</t>
+  </si>
+  <si>
+    <t>metadata</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MetaboliteMethod </t>
+  </si>
+  <si>
+    <t>MetaboliteRecoveryCorrectionApplied</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DispersionCorrected </t>
+  </si>
+  <si>
+    <t>HPLC</t>
   </si>
 </sst>
 </file>
@@ -536,10 +551,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4D07A739-95C2-BD46-B2B0-50E40D980EB4}">
-  <dimension ref="A1:AC26"/>
+  <dimension ref="A1:AD26"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="X1" workbookViewId="0">
-      <selection activeCell="AA14" sqref="AA14"/>
+      <selection activeCell="AB10" sqref="AB10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
@@ -566,16 +581,17 @@
     <col min="21" max="21" width="17.58203125" style="2" bestFit="1" customWidth="1"/>
     <col min="22" max="22" width="26.58203125" style="2" bestFit="1" customWidth="1"/>
     <col min="23" max="23" width="25.6640625" style="2" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="16.5" style="2" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="11.75" style="2" bestFit="1" customWidth="1"/>
     <col min="25" max="25" width="19.08203125" style="2" bestFit="1" customWidth="1"/>
     <col min="26" max="26" width="14" style="2" bestFit="1" customWidth="1"/>
     <col min="27" max="27" width="21.1640625" style="2" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="16" style="2" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="23.33203125" style="2" bestFit="1" customWidth="1"/>
-    <col min="30" max="16384" width="10.6640625" style="2"/>
+    <col min="28" max="28" width="33" style="2" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="16" style="2" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="23.33203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="31" max="16384" width="10.6640625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:29" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -658,13 +674,16 @@
         <v>40</v>
       </c>
       <c r="AB1" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="AC1" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="AC1" s="1" t="s">
+      <c r="AD1" s="1" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="2" spans="1:29" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
         <v>23</v>
       </c>
@@ -746,14 +765,17 @@
       <c r="AA2" s="2">
         <v>2.4202870927432429</v>
       </c>
-      <c r="AB2" s="2">
+      <c r="AB2" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="AC2" s="2">
         <v>0.1</v>
       </c>
-      <c r="AC2" s="2">
+      <c r="AD2" s="2">
         <v>0.1806712347038926</v>
       </c>
     </row>
-    <row r="3" spans="1:29" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:30" x14ac:dyDescent="0.35">
       <c r="P3" s="2">
         <v>60</v>
       </c>
@@ -772,14 +794,17 @@
       <c r="AA3" s="2">
         <v>2.0191223235726747</v>
       </c>
-      <c r="AB3" s="2">
+      <c r="AB3" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="AC3" s="2">
         <v>0.2</v>
       </c>
-      <c r="AC3" s="2">
+      <c r="AD3" s="2">
         <v>0.12315723878982274</v>
       </c>
     </row>
-    <row r="4" spans="1:29" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:30" x14ac:dyDescent="0.35">
       <c r="P4" s="2">
         <v>180</v>
       </c>
@@ -798,14 +823,17 @@
       <c r="AA4" s="2">
         <v>1.3336153655648415</v>
       </c>
-      <c r="AB4" s="2">
+      <c r="AB4" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="AC4" s="2">
         <v>0.3</v>
       </c>
-      <c r="AC4" s="2">
+      <c r="AD4" s="2">
         <v>0.13827082850410888</v>
       </c>
     </row>
-    <row r="5" spans="1:29" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:30" x14ac:dyDescent="0.35">
       <c r="P5" s="2">
         <v>540</v>
       </c>
@@ -824,14 +852,17 @@
       <c r="AA5" s="2">
         <v>0.71375630065532591</v>
       </c>
-      <c r="AB5" s="2">
+      <c r="AB5" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="AC5" s="2">
         <v>0.4</v>
       </c>
-      <c r="AC5" s="2">
+      <c r="AD5" s="2">
         <v>1.5586366435794305</v>
       </c>
     </row>
-    <row r="6" spans="1:29" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:30" x14ac:dyDescent="0.35">
       <c r="P6" s="2">
         <v>1260</v>
       </c>
@@ -850,172 +881,179 @@
       <c r="AA6" s="2">
         <v>0.40944545194439969</v>
       </c>
-      <c r="AB6" s="2">
+      <c r="AB6" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="AC6" s="2">
         <v>0.5</v>
       </c>
-      <c r="AC6" s="2">
+      <c r="AD6" s="2">
         <v>12.60661967715952</v>
       </c>
     </row>
-    <row r="7" spans="1:29" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:30" x14ac:dyDescent="0.35">
       <c r="P7" s="2">
         <v>2700</v>
       </c>
       <c r="Q7" s="2">
         <v>300</v>
       </c>
-      <c r="AB7" s="2">
+      <c r="AB7" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="AC7" s="2">
         <v>0.6</v>
       </c>
-      <c r="AC7" s="2">
+      <c r="AD7" s="2">
         <v>21.642328472165822</v>
       </c>
     </row>
-    <row r="8" spans="1:29" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:30" x14ac:dyDescent="0.35">
       <c r="P8" s="2">
         <v>4500</v>
       </c>
       <c r="Q8" s="2">
         <v>300</v>
       </c>
-      <c r="AB8" s="2">
+      <c r="AC8" s="2">
         <v>0.7</v>
       </c>
-      <c r="AC8" s="2">
+      <c r="AD8" s="2">
         <v>28.260412432814505</v>
       </c>
     </row>
-    <row r="9" spans="1:29" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:30" x14ac:dyDescent="0.35">
       <c r="P9" s="2">
         <v>6300</v>
       </c>
       <c r="Q9" s="2">
         <v>300</v>
       </c>
-      <c r="AB9" s="2">
+      <c r="AC9" s="2">
         <v>0.8</v>
       </c>
-      <c r="AC9" s="2">
+      <c r="AD9" s="2">
         <v>25.732606124169475</v>
       </c>
     </row>
-    <row r="10" spans="1:29" x14ac:dyDescent="0.35">
-      <c r="AB10" s="2">
+    <row r="10" spans="1:30" x14ac:dyDescent="0.35">
+      <c r="AC10" s="2">
         <v>0.9</v>
       </c>
-      <c r="AC10" s="2">
+      <c r="AD10" s="2">
         <v>19.430288690813679</v>
       </c>
     </row>
-    <row r="11" spans="1:29" x14ac:dyDescent="0.35">
-      <c r="AB11" s="2">
+    <row r="11" spans="1:30" x14ac:dyDescent="0.35">
+      <c r="AC11" s="2">
         <v>1</v>
       </c>
-      <c r="AC11" s="2">
+      <c r="AD11" s="2">
         <v>15.763897581969536</v>
       </c>
     </row>
-    <row r="12" spans="1:29" x14ac:dyDescent="0.35">
-      <c r="AB12" s="2">
+    <row r="12" spans="1:30" x14ac:dyDescent="0.35">
+      <c r="AC12" s="2">
         <v>5</v>
       </c>
-      <c r="AC12" s="2">
+      <c r="AD12" s="2">
         <v>2.6038257396855387</v>
       </c>
     </row>
-    <row r="13" spans="1:29" x14ac:dyDescent="0.35">
-      <c r="AB13" s="2">
+    <row r="13" spans="1:30" x14ac:dyDescent="0.35">
+      <c r="AC13" s="2">
         <v>5.0999999999999996</v>
       </c>
-      <c r="AC13" s="2">
+      <c r="AD13" s="2">
         <v>1.4127075293008573</v>
       </c>
     </row>
-    <row r="14" spans="1:29" x14ac:dyDescent="0.35">
-      <c r="AB14" s="2">
+    <row r="14" spans="1:30" x14ac:dyDescent="0.35">
+      <c r="AC14" s="2">
         <v>5.2</v>
       </c>
-      <c r="AC14" s="2">
+      <c r="AD14" s="2">
         <v>1.5508024213271285</v>
       </c>
     </row>
-    <row r="15" spans="1:29" x14ac:dyDescent="0.35">
-      <c r="AB15" s="2">
+    <row r="15" spans="1:30" x14ac:dyDescent="0.35">
+      <c r="AC15" s="2">
         <v>5.3</v>
       </c>
-      <c r="AC15" s="2">
+      <c r="AD15" s="2">
         <v>1.9835303309212777</v>
       </c>
     </row>
-    <row r="16" spans="1:29" x14ac:dyDescent="0.35">
-      <c r="AB16" s="2">
+    <row r="16" spans="1:30" x14ac:dyDescent="0.35">
+      <c r="AC16" s="2">
         <v>5.4</v>
       </c>
-      <c r="AC16" s="2">
+      <c r="AD16" s="2">
         <v>1.2821724442055766</v>
       </c>
     </row>
-    <row r="17" spans="25:29" x14ac:dyDescent="0.35">
-      <c r="AB17" s="2">
+    <row r="17" spans="25:30" x14ac:dyDescent="0.35">
+      <c r="AC17" s="2">
         <v>5.5</v>
       </c>
-      <c r="AC17" s="2">
+      <c r="AD17" s="2">
         <v>1.9230837535950536</v>
       </c>
     </row>
-    <row r="18" spans="25:29" x14ac:dyDescent="0.35">
-      <c r="AB18" s="2">
+    <row r="18" spans="25:30" x14ac:dyDescent="0.35">
+      <c r="AC18" s="2">
         <v>5.6</v>
       </c>
-      <c r="AC18" s="2">
+      <c r="AD18" s="2">
         <v>1.8590866181962005</v>
       </c>
     </row>
-    <row r="19" spans="25:29" x14ac:dyDescent="0.35">
-      <c r="AB19" s="2">
+    <row r="19" spans="25:30" x14ac:dyDescent="0.35">
+      <c r="AC19" s="2">
         <v>5.7</v>
       </c>
-      <c r="AC19" s="2">
+      <c r="AD19" s="2">
         <v>1.5760483803048748</v>
       </c>
     </row>
-    <row r="20" spans="25:29" x14ac:dyDescent="0.35">
-      <c r="AB20" s="2">
+    <row r="20" spans="25:30" x14ac:dyDescent="0.35">
+      <c r="AC20" s="2">
         <v>5.8</v>
       </c>
-      <c r="AC20" s="2">
+      <c r="AD20" s="2">
         <v>1.5079092518548047</v>
       </c>
     </row>
-    <row r="21" spans="25:29" x14ac:dyDescent="0.35">
-      <c r="AB21" s="2">
+    <row r="21" spans="25:30" x14ac:dyDescent="0.35">
+      <c r="AC21" s="2">
         <v>5.9</v>
       </c>
-      <c r="AC21" s="2">
+      <c r="AD21" s="2">
         <v>1.8746585867777545</v>
       </c>
     </row>
-    <row r="22" spans="25:29" x14ac:dyDescent="0.35">
-      <c r="AB22" s="2">
+    <row r="22" spans="25:30" x14ac:dyDescent="0.35">
+      <c r="AC22" s="2">
         <v>6</v>
       </c>
-      <c r="AC22" s="2">
+      <c r="AD22" s="2">
         <v>1.4461300767213285</v>
       </c>
     </row>
-    <row r="23" spans="25:29" x14ac:dyDescent="0.35">
+    <row r="23" spans="25:30" x14ac:dyDescent="0.35">
       <c r="Y23" s="4"/>
     </row>
-    <row r="24" spans="25:29" x14ac:dyDescent="0.35">
+    <row r="24" spans="25:30" x14ac:dyDescent="0.35">
       <c r="Y24" s="4"/>
     </row>
-    <row r="25" spans="25:29" x14ac:dyDescent="0.35">
+    <row r="25" spans="25:30" x14ac:dyDescent="0.35">
       <c r="Y25" s="4"/>
     </row>
-    <row r="26" spans="25:29" x14ac:dyDescent="0.35">
+    <row r="26" spans="25:30" x14ac:dyDescent="0.35">
       <c r="Y26" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>